<commit_message>
New items is added.
</commit_message>
<xml_diff>
--- a/food_details.xlsx
+++ b/food_details.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Android_Client_Projects\MoroccanCuisine\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8155E1C1-609E-4629-9730-93760FFBCCB5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{366D633B-CDE8-464F-8376-71D28C7554A7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{7E3379E6-54C8-4964-AA0C-E9C7B352179A}"/>
   </bookViews>
@@ -31,57 +31,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
-  <si>
-    <t>18 ingrédients
-Viandes
-400 g Lamb neck, fillet
-1 Lamb stock cube
-Fruits et légumes
-1 400g tin Chickpeas
-1 tsp Coriander, ground
-1 30g pack Coriander
-75 g Dried apricots
-1 Garlic clove
-1 Onion
-Conserves
-1 Chicken stock cube
-Condiments
-1 tbsp Clear honey
-Pâtes et céréales
-150 g Couscous
-Aides culinaires et épices
-1 tsp Cinnamon, ground
-1/2 tsp Paprika, smoked
-1 Red pepper
-1 tsp Turmeric
-Huiles et vinaigres
-1 tbsp Olive oil
-Fruits secs et graines
-25 g Almonds, flaked
-1 tsp Cumin, ground</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="72">
   <si>
     <t>Lamb Tagine</t>
   </si>
   <si>
     <t>Loubia marocaine</t>
-  </si>
-  <si>
-    <t>Ingrédients / pour 4 personnes
-250 g de haricots blancs trempés la veille
-300g de viande de bœuf
-1 oignon haché
-2 tomates concassées (ou 200ml de purée de tomate)
-2 cuillère à café de concentré de tomate
-2 carottes en rondelles
-3 cuillères à soupe d'huile d'olive
-1 gousse d'ail (ou une cuillère à café d'ail en poudre)
-1 cuillère à soupe de gingembre moulu
-1/2 cuillère à café de cumin
-1 feuille de laurier
-Sel et poivre
-Eau</t>
   </si>
   <si>
     <t>Tajine au poulet</t>
@@ -267,19 +222,551 @@
     <t>Zaalouk</t>
   </si>
   <si>
-    <t>Ingrédients :
-3 aubergines moyennes
-3 gousses d’ail
-4 cuillères à soupe d’huile d’olive extra vierge
-3 tomates bien mûres, pelées et hachées
-1 cuillère à café de paprika doux
-1 cuillère à café de cumin moulu
-1 pincée de piment fort
-1/4 de cuillère à café de curcuma
-Du sel et du poivre
-2 cuillères à soupe de coriandre fraîche finement hachée
-1 cuillère à soupe de persil plat finement haché
-Quelques olives violettes (facultatif)</t>
+    <t>Baked falafels # vegan</t>
+  </si>
+  <si>
+    <t>or about twenty falafels:
+• 250 g of dried chickpeas
+• 1 onion
+• 2 cloves garlic
+• 1/2 bunch of flat-leaf parsley
+• 1/2 bunch of coriander (or 1 tbsp ground coriander)
+• 1 tbsp of tahini (or sesame seed)
+• 2 tsp of cumin
+• 1 tsp of baking soda
+• 1/2 tsp of Espelette pepper
+For the side sauce:
+• 10 cl of soy cream (or 1 Greek yogurt)
+• 1 rounded tbsp of tahini
+• 1 tbsp of lemon juice
+• 1 clove of garlic</t>
+  </si>
+  <si>
+    <t>Baked tomatoes</t>
+  </si>
+  <si>
+    <t>For 4 people
+16 tomatoes
+1 tablespoon of garlic powder
+4 tablespoons of olive oil
+2 tablespoons of herbs (rosemary, thyme, Provence, ...)
+1 teaspoon of powdered sugar
+1 pinch of salt,
+1 pinch of pepper
+Cut your tomatoes in 2.
+Place them face up in a dish. Sprinkle with powdered garlic, salt, pepper, herbs (if you like). Drizzle with olive oil and sprinkle with a little powdered sugar.
+Cook for at least 2 hours in a low oven (120 / 150ºC).</t>
+  </si>
+  <si>
+    <t>Bissara</t>
+  </si>
+  <si>
+    <t>Ingredients
+500 g split peas
+6 garlic cloves (4 garlic cloves)
+salt
+paprika
+1 tsp of cumin
+Olive oil
+hot pepper
+Sufficient amount of water
+Instructions
+In a deep-bottomed saucepan add the split peas as well as the garlic cloves and spices.
+Pour water. cover and cook (about 30 minutes)
+Once cooked, remove the pan from the heat and let cool. Mix with a hand blender
+Serve immediately, drizzling with olive oil and sprinkling with paprika and cumin.</t>
+  </si>
+  <si>
+    <t>Carrot, peas and potato tagine</t>
+  </si>
+  <si>
+    <t>15 ingredients
+Ingredients
+3 pieces of meat (less than 300g)
+1 onion
+2 potatoes
+1 carrot
+3 handfuls of frozen peas and carrots
+1 tsp of salt
+1 tsp of paprika
+1 tsp of ginger
+1 tsp of turmeric
+1/2 tsp of pepper
+1 garlic clove, grated
+1 meat broth
+Olive oil
+Sunflower oil
+Parsley</t>
+  </si>
+  <si>
+    <t>Chermoula fish tagine</t>
+  </si>
+  <si>
+    <t>13 ingredients
+Meats
+1 A dash of lemon juice
+Fruits and vegetables
+12 cloves of garlic
+Condiments
+1 Olive oil
+1 Green and purple olives
+Culinary aids and spices
+2 cup of paprika
+Dried fruits and seeds
+2 cup cumin
+Other
+2 Beautiful red tomatoes, cut into slices
+1 tsp of pepper
+1 Royal sea bream
+2 medium onions, cut into thin strips
+Salt
+A bunch of parsley and cilantro
+For the chermoula:</t>
+  </si>
+  <si>
+    <t>Chicken tagine</t>
+  </si>
+  <si>
+    <t>18 ingredients
+Ingredients
+1 whole chicken cut into pieces
+1 grated onion
+1 grated tomato
+3 potatoes
+3 garlic cloves, chopped
+1/2 candied lemon, cut into small pieces
+100 g green olives
+1 glass (s) of water
+1 teaspoon of salt
+1 teaspoon (s) of turmeric
+1/2 teaspoon (s) of cinnamon
+1 teaspoon (s) of ginger
+1/2 teaspoon (s) of pepper
+3 tablespoon (s) of chopped cilantro
+3 tablespoon (s) of chopped parsley
+1 teaspoon (s) of saffron
+2 tablespoon (s) of olive oil
+1 tablespoon (s) of vegetable oil</t>
+  </si>
+  <si>
+    <t>Chicken tagine with almonds</t>
+  </si>
+  <si>
+    <t>11 ingredients
+Meats
+1 Beautiful cut chicken
+Fruits and vegetables
+1 clove of garlic
+1 The juice of 1 lemon
+Other
+1 bunch of coriander
+1/2 bunch of parsley
+1 Teaspoon (s) of ground ginger
+4 tablespoon (s) of peanut oil
+100 g of blanched almonds
+400 g Onions
+1 Dose of saffron powder
+salt pepper</t>
+  </si>
+  <si>
+    <t>Chicken tagine with apricots, prunes and toasted almonds</t>
+  </si>
+  <si>
+    <t>Ingredients for 5 people
+Time: 30 minutes of preparation + 1 night in the refrigerator + 1 h 30
+2 onions, finely chopped
+3 to 4 garlic cloves, finely chopped
+Fresh cilantro, finely chopped
+ ½ bunch of flat-leaf parsley, finely chopped
+ 4 tbsp olive oil
+ ½ lemon, juice only
+ Salt and freshly ground black pepper
+ 2 tsp ground ginger
+ 5 tsp ground cinnamon
+ ½ tsp ground turmeric
+ 10 chicken thighs or drumsticks
+ 1 chicken stock cube
+ 150 g of dried prunes
+ 3 tbsp caster sugar
+ 150g of dried apricots
+ 100g of white almonds, toasted
+Serve with
+Baked semolina or bread</t>
+  </si>
+  <si>
+    <t>From Vegetables  Tajine</t>
+  </si>
+  <si>
+    <t>4 medium potatoes
+2 carrots
+2 courgettes
+2 tomatoes
+2 peppers
+1/2 small butternut squash
+1 onion
+1 garlic clove
+10 green olives
+4 prunes
+parsley and coriander
+salt and pepper
+1 C. 1/2 teaspoon ground ginger
+1 C. teaspoon of turmeric
+1 C. 1/2 teaspoon ground cumin
+1/2 tsp. 1/2 teaspoon ground coriander
+4 c. tablespoon olive oil</t>
+  </si>
+  <si>
+    <t>From Vegetables Tajine</t>
+  </si>
+  <si>
+    <t>10 ingredients
+Meats
+1/2 candied lemon
+Fruits and vegetables
+2 Eggplants of about, small
+1 courgette
+1 Small rutabaga, about 340 g (3/4 lb)
+Other
+1/2 teaspoon (2.5 ml) ground cumin
+500 ml (2 cups) vegetable or chicken broth
+1 540 ml (19 oz) can chickpeas, rinsed and drained
+1 Red bell pepper, seeded and cut into strips
+15 ml (1 tbsp.) Homemade harissa paste (see recipe) or store-bought
+50 g (1/4 cup) dried apricots, cut into 4</t>
+  </si>
+  <si>
+    <t>From Vegetables Tajine1</t>
+  </si>
+  <si>
+    <t>Ingredients:
+- 2 carrots cut in 4
+- 2 courgettes cut in 4
+- 2 to 3 potatoes, cut in half lengthwise
+- a few strips of pepper
+- 2 to 3 sliced ??tomatoes
+- a small bowl of peas (frozen for me)
+- a small piece of meat of your choice (here a chicken thigh cut in 2)
+- a bunch of chopped parsley and coriander
+- a handful of olives
+- 4 garlic cloves, chopped
+- 1/3 candied lemon in pieces
+- salt pepper
+- a small tea glass of olive oil
+ spices :
+- ginger
+- turmeric
+- mild red pepper
+cumin</t>
+  </si>
+  <si>
+    <t>Luciana-style octopus</t>
+  </si>
+  <si>
+    <t>Ingredients
+1 kg of clean small octopus
+4-5- peeled tomatoes
+1/2 tablespoon of salted capers
+100  g of black Gaeta olives
+1 sprig of parsley
+hot pepper to taste
+2 cloves of garlic
+extra virgin olive oil and salt to taste</t>
+  </si>
+  <si>
+    <t>Meatball and potato tagine</t>
+  </si>
+  <si>
+    <t>14 ingredients
+Meats
+500 g minced beef
+1 drizzle of olive oil
+Fruits and vegetables
+2 cloves garlic
+Condiments
+1 medium white or red onion
+1 A few rinsed and drained olives
+Culinary aids and spices
+1 tablespoon of paprika
+Dried fruits and seeds
+1/2 teaspoon ground cumin
+Other
+1 bunch of parsley (or cilantro, or half and half)
+1 teaspoon of powdered ginger
+½ teaspoon chilli powder (optional)
+Fresh or dry mint (optional)
+6 medium potatoes
+Salt and freshly ground pepper to taste
+1 Cup | 250 ml of peeled and crushed tomatoes (I used canned tomatoes)</t>
+  </si>
+  <si>
+    <t>Moroccan Fish Tagine</t>
+  </si>
+  <si>
+    <t>1 kg fish (wolf)
+2 tbsp Parsley and coriander
+3 cloves of garlic
+1.5 lemon juice
+2 Peppers (green, red)
+4 Carrots, peeled and cut into thin slices
+3 tbsp Tomato sauce
+1/2 glass of olive oil
+1 small glass of water
+1 tsp Cumin
+1 tsp Paprika
+Salt pepper</t>
+  </si>
+  <si>
+    <t>Moroccan lentils</t>
+  </si>
+  <si>
+    <t>Ingredients:
+250 g of well cleaned and washed lentils.
+1 chopped tomato
+1 chopped onions
+1 garlic clove, grated
+1/4 tsp ginger
+1/4 tsp cumin
+1/2 tsp turmeric
+1 little pepper
+1/2 tsp paprika
+1 tsp of salt
+1 little chilli (optional if you don't like chili)
+1 tsp filled with tomato paste
+1 tbsp of parsley
+olive oil
+water for cooking</t>
+  </si>
+  <si>
+    <t>Mutton tagine</t>
+  </si>
+  <si>
+    <t>9 ingrédients
+Ingrédients
+1.5 kg d'agneau
+2 oignons
+6 pommes de terre
+6 tomates
+4 pêches ou brugnons (frais ou en boîte selon l'époque)
+amandes effilées
+12 pruneaux
+1 bouillon Kub
+épices safran, coriandre en graines, fleur d'oranger, pimen</t>
+  </si>
+  <si>
+    <t>Potato and minced meat tagine</t>
+  </si>
+  <si>
+    <t>Ingredients:
+250g minced meat
+a big potato
+an onion
+a big tomato
+1 tsp of tomato paste
+2 cloves garlic
+salt / pepper / paprika / cumin / turmeric
+parsley and chopped cilantro
+a sweet or hot pepper
+olive oil
+Water</t>
+  </si>
+  <si>
+    <t>Sardine tagine</t>
+  </si>
+  <si>
+    <t>500 gr sardines
+cumin
+turmeric
+paprika
+pepper
+salt
+1 glass of cooked rice
+1 egg white
+3 tomatoes
+2 cloves garlic
+3 gr.c parsley
+3 gr.c olive oil
+1 green pepper
+1 red pepper
+lemon confit</t>
+  </si>
+  <si>
+    <t>Tagine with prunes and dried apricots</t>
+  </si>
+  <si>
+    <t>For this recipe, you will need: for 4 people
+- beef shank
+- 2 onions
+- olive oil
+- salt and pepper
+- 1/2 teaspoon ground ginger
+- 1 tsp of turmeric
+- 1 pinch of pure saffron
+- cinnamon powder
+- 2 cinnamon sticks
+- ten prunes
+- about ten dried apricots
+- 3 tbsp of powdered sugar
+- ten almonds
+- sesame seeds</t>
+  </si>
+  <si>
+    <t>Tajine aux petits pois et aux oeufs</t>
+  </si>
+  <si>
+    <t>ingredients
+a bowl of fresh or frozen peas or a can of canned peas
+a finely chopped onion
+a good tbsp of tomato paste diluted in a small glass of water
+2 garlic cloves, crushed
+1 tbsp of chopped parsley
+1 tsp of cumin
+salt
+2 tbsp olive oil
+4 eggs
+chopped parsley and cumin for the end</t>
+  </si>
+  <si>
+    <t>Turkey tagine with fennel</t>
+  </si>
+  <si>
+    <t>12 ingredients
+Fruits and vegetables
+2 cloves garlic
+Preserves
+1 chicken broth fat
+Other
+1 fennel bulb
+coriander powder
+fresh coriander
+turmeric
+350 g Turkey cutlets
+ginger
+2 Cardamom pods
+1 red onion
+ras el hanout
+salt</t>
+  </si>
+  <si>
+    <t>Vegetable tagine with wild peach and pistachio</t>
+  </si>
+  <si>
+    <t>13 ingredients
+Pâtes et céréales
+275 g Organic couscous
+Autre
+0.5 tsp ground cinnamon
+1 can of chickpeas (410 g)
+1 can of tomato cubes (400 g)
+3 tbsp salted pistachios
+2 Tbsp olive oil
+1 Possibly. tajine
+1 pinch of pepper
+2 sprigs of mint
+1 tsp ground cumin
+1 Onion
+2 Wild peaches
+1 Carrot</t>
+  </si>
+  <si>
+    <t>Vegetarian tagine with prunes</t>
+  </si>
+  <si>
+    <t>14 ingredients
+Ingredients
+500 g green beans
+20 prunes
+4 carrots
+4 turnips
+3 courgettes
+1 onion
+1/2 bunch of parsley
+1/2 bunch of coriander
+2 tbsp. tablespoons of olive oil
+1 C. coffee from ras el hanout
+1 C. 1/2 teaspoon ground ginger
+1 C. ground turmeric
+1 C. teaspoon paprika
+Salt pepper</t>
+  </si>
+  <si>
+    <t>Winter vegetable and dried fruit tagine</t>
+  </si>
+  <si>
+    <t>For 4 to 6 people
+ 1 pumpkin quarter 
+ 2 carrots
+ 1 large rutabaga (or 2 medium) that can be replaced by turnip
+ 12 Agen prunes
+ 12 dried apricots
+ 2 tablespoons of ground cinnamon
+ 1 cinnamon stick
+ 2 tablespoons of powdered ginger
+ 1 tablespoon of turmeric - 1 tablespoon of paprika
+ 1 tablespoon of ras-el-hanout - salt, pepper
+ 2 teaspoon of powdered sugar - 1 large onion ( or 2 small!)
+ 2 cloves of garlic - 30cl of lukewarm water
+ 2 handfuls of chickpeas (I didn't have any anymore) 
+ fresh cilantro (no more)</t>
+  </si>
+  <si>
+    <t>Ingredients:
+3 medium eggplants
+3 cloves of garlic
+4 tablespoons of extra virgin olive oil
+3 ripe tomatoes, peeled and chopped
+1 teaspoon of sweet paprika
+1 teaspoon of ground cumin
+1 pinch of hot pepper
+1/4 teaspoon of turmeric
+Salt and pepper
+2 tablespoons finely chopped fresh cilantro
+1 tablespoon finely chopped flat-leaf parsley
+A few purple olives (optional)</t>
+  </si>
+  <si>
+    <t>18 ingredients
+Meats
+400 g Lamb neck, fillet
+1 Lamb stock cube
+Fruits and vegetables
+1 400g tin Chickpeas
+1 tsp Coriander, ground
+1 30g Coriander pack
+75 g Dried apricots
+1 Garlic clove
+1 Onion
+Preserves
+1 Chicken stock cube
+Condiments
+1 tbsp Clear honey
+Pasta and cereals
+150 g Couscous
+Culinary aids and spices
+1 tsp Cinnamon, ground
+1/2 tsp Paprika, smoked
+1 Red pepper
+1 tsp Turmeric
+Oils and vinegars
+1 tbsp Olive oil
+Dried fruits and seeds
+25 g Almonds, flaked
+1 tsp Cumin, ground</t>
+  </si>
+  <si>
+    <t>Ingredients for 4 persons
+250 g white beans soaked the day before
+300g of beef
+1 chopped onion
+2 crushed tomatoes (or 200ml tomato puree)
+2 teaspoon of tomato paste
+2 sliced ??carrots
+3 tablespoons of olive oil
+1 clove of garlic (or a teaspoon of garlic powder)
+1 tablespoon of ground ginger
+1/2 teaspoon of cumin
+1 bay leaf
+Salt and pepper
+Water</t>
   </si>
 </sst>
 </file>
@@ -637,112 +1124,304 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41AE60DC-381B-4C01-8EFA-723016B85013}">
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:B36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="50.85546875" style="2" customWidth="1"/>
+    <col min="1" max="1" width="59.42578125" style="2" customWidth="1"/>
     <col min="2" max="2" width="32.42578125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="405" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="270" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="255" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="315" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="270" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="330" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="345" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="225" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="345" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="270" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="315" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="375" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="405" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="255" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="285" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="B13" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="390" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="195" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="270" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="195" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="210" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="225" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="240" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="210" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="375" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B23" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="375" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+    <row r="24" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B24" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B25" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+    </row>
+    <row r="26" spans="1:2" ht="330" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B26" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="330" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+    </row>
+    <row r="27" spans="1:2" ht="255" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B27" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="255" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+    <row r="28" spans="1:2" ht="195" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B28" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="195" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
+    <row r="29" spans="1:2" ht="255" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B29" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="255" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
+    <row r="30" spans="1:2" ht="225" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B30" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="225" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
+    <row r="31" spans="1:2" ht="240" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B31" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="240" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
+    <row r="32" spans="1:2" ht="240" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" ht="240" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" ht="240" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" ht="330" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" ht="255" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" ht="270" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>23</v>
+      <c r="B36" s="1" t="s">
+        <v>69</v>
       </c>
     </row>
   </sheetData>

</xml_diff>